<commit_message>
- parse the resulting datatable
</commit_message>
<xml_diff>
--- a/POC_Excel/Lista studenti.xlsx
+++ b/POC_Excel/Lista studenti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toni\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toni\Desktop\POC_Excel\POC_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75425562-A82B-476F-B78F-0B06A267AD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551683F0-A8DF-441D-BDD1-9FF0515C2C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{82A90A5D-1011-4C2C-B6D7-08E8DAAB7DEE}"/>
+    <workbookView xWindow="6540" yWindow="600" windowWidth="21600" windowHeight="11145" xr2:uid="{82A90A5D-1011-4C2C-B6D7-08E8DAAB7DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Foaie1" sheetId="1" r:id="rId1"/>
@@ -39,12 +39,6 @@
     <t>Nume</t>
   </si>
   <si>
-    <t>Nr.</t>
-  </si>
-  <si>
-    <t>Facultatea</t>
-  </si>
-  <si>
     <t>Pitic Antoniu</t>
   </si>
   <si>
@@ -61,6 +55,12 @@
   </si>
   <si>
     <t>Facultatea de Litere</t>
+  </si>
+  <si>
+    <t>Nr</t>
+  </si>
+  <si>
+    <t>Facultate</t>
   </si>
 </sst>
 </file>
@@ -415,48 +415,48 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>